<commit_message>
Localization.tsv is now automatically to C++ printf format.
</commit_message>
<xml_diff>
--- a/Localization/Translation Master.xlsx
+++ b/Localization/Translation Master.xlsx
@@ -11004,8 +11004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K349"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>